<commit_message>
everything is hook up and running
</commit_message>
<xml_diff>
--- a/moduler/toolmonitor_data/results/RawDatabase.xlsx
+++ b/moduler/toolmonitor_data/results/RawDatabase.xlsx
@@ -448,7 +448,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>S49</t>
+          <t>S38</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -520,7 +520,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>S226</t>
+          <t>S219</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -664,7 +664,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>S37</t>
+          <t>S36</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>S36</t>
+          <t>S44</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -880,7 +880,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>S41</t>
+          <t>S36</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -972,7 +972,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>S10000000</t>
+          <t>S00000000</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S22</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>S14</t>
+          <t>S18</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>S10000000</t>
+          <t>S00000000</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>S77</t>
+          <t>S72</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>S41</t>
+          <t>S40</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1888,12 +1888,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>S178404</t>
+          <t>S177808</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1955,7 +1955,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>S60</t>
+          <t>S100</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>S151174</t>
+          <t>S158130</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -2104,12 +2104,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>S164</t>
+          <t>S137</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>S165559</t>
+          <t>S159297</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>S58</t>
+          <t>S47</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>S15</t>
+          <t>S14</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2680,7 +2680,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>S4</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>S16</t>
+          <t>S15</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -2968,7 +2968,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3040,7 +3040,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>S37</t>
+          <t>S36</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3112,12 +3112,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>S4</t>
+          <t>S25</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>S218809</t>
+          <t>S213882</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -3256,7 +3256,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>S21</t>
+          <t>S20</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>S35</t>
+          <t>S33</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S19</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3904,7 +3904,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>S12</t>
+          <t>S11</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -3971,17 +3971,17 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>S10</t>
+          <t>S20</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S19</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>S197915</t>
+          <t>S197446</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -4192,7 +4192,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>S33</t>
+          <t>S29</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4408,12 +4408,12 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>S34</t>
+          <t>S37</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>S211999</t>
+          <t>S211952</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -4480,7 +4480,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S7</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4552,7 +4552,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S28</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4624,7 +4624,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S7</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4696,7 +4696,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>S6</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -4984,7 +4984,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>S22</t>
+          <t>S20</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5056,7 +5056,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>S34</t>
+          <t>S30</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5416,7 +5416,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>S90</t>
+          <t>S89</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5560,7 +5560,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>S34</t>
+          <t>S26</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5632,7 +5632,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>S4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5776,7 +5776,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>S46</t>
+          <t>S35</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -5920,12 +5920,12 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>S46</t>
+          <t>S45</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>S226909</t>
+          <t>S224644</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -5992,7 +5992,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>S32</t>
+          <t>S30</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6064,7 +6064,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>S7</t>
+          <t>S6</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6856,7 +6856,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>S27</t>
+          <t>S15</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -7005,7 +7005,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>S169886</t>
+          <t>S137515</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -7072,7 +7072,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>S99</t>
+          <t>S98</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -7144,7 +7144,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>S19</t>
+          <t>S18</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -7211,17 +7211,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S180</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S146</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>S176106</t>
+          <t>S138724</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>S36</t>
+          <t>S34</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -7432,7 +7432,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>S15</t>
+          <t>S14</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -7576,7 +7576,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>S29</t>
+          <t>S8</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -7648,7 +7648,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>S94</t>
+          <t>S60</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -7720,7 +7720,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>S243</t>
+          <t>S162</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -7792,7 +7792,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -7931,17 +7931,17 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S180</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S118</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>S204993</t>
+          <t>S150270</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -8008,7 +8008,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>S10</t>
+          <t>S9</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -8085,7 +8085,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>S155169</t>
+          <t>S187764</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -8152,7 +8152,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>S28</t>
+          <t>S22</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -8229,7 +8229,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>S189193</t>
+          <t>S188858</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -8296,7 +8296,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>S10</t>
+          <t>S8</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -8512,7 +8512,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>S55</t>
+          <t>S36</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -8944,7 +8944,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S13</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -9021,7 +9021,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>S163004</t>
+          <t>S182026</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
@@ -9165,7 +9165,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>S267032</t>
+          <t>S172127</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -9381,7 +9381,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>S200005</t>
+          <t>S198650</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -9520,7 +9520,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>S31</t>
+          <t>S24</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -9755,7 +9755,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>S48</t>
+          <t>S38</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -9827,7 +9827,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>S226</t>
+          <t>S219</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -9971,7 +9971,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>S37</t>
+          <t>S36</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -10115,7 +10115,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>S11</t>
+          <t>S44</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -10187,7 +10187,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>S37</t>
+          <t>S36</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -10279,7 +10279,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>S10000000</t>
+          <t>S00000000</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -10691,7 +10691,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S22</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -10763,7 +10763,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>S14</t>
+          <t>S18</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -10979,7 +10979,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -10999,7 +10999,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>S10000000</t>
+          <t>S00000000</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -11051,7 +11051,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>S77</t>
+          <t>S72</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -11123,7 +11123,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>S41</t>
+          <t>S40</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -11195,12 +11195,12 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>S4</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>S178404</t>
+          <t>S177808</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -11262,17 +11262,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>S60</t>
+          <t>S100</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>S12</t>
+          <t>S14</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>S151174</t>
+          <t>S158130</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -11411,12 +11411,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>S133</t>
+          <t>S137</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>S165559</t>
+          <t>S159297</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -11843,7 +11843,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>S55</t>
+          <t>S47</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -11915,7 +11915,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>S15</t>
+          <t>S14</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -11987,7 +11987,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -12275,7 +12275,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -12347,7 +12347,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>S37</t>
+          <t>S36</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -12419,12 +12419,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>S25</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>S218809</t>
+          <t>S213882</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -12563,7 +12563,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>S21</t>
+          <t>S20</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -12707,7 +12707,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>S35</t>
+          <t>S33</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -12995,7 +12995,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S19</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -13211,7 +13211,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>S12</t>
+          <t>S11</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -13278,17 +13278,17 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>S10</t>
+          <t>S20</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S19</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>S197915</t>
+          <t>S197446</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -13499,7 +13499,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>S33</t>
+          <t>S29</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -13715,12 +13715,12 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>S34</t>
+          <t>S37</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>S211999</t>
+          <t>S211952</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -13787,7 +13787,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S7</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -13859,7 +13859,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>S8</t>
+          <t>S28</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -13931,7 +13931,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S7</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -14291,7 +14291,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>S21</t>
+          <t>S20</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -14363,7 +14363,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>S34</t>
+          <t>S30</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -14723,7 +14723,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>S90</t>
+          <t>S89</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -14867,7 +14867,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>S34</t>
+          <t>S26</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -14939,7 +14939,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>S4</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -15083,7 +15083,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>S44</t>
+          <t>S35</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -15227,12 +15227,12 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>S46</t>
+          <t>S45</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>S226909</t>
+          <t>S224644</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -15299,7 +15299,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>S31</t>
+          <t>S30</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -15371,7 +15371,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>S7</t>
+          <t>S6</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -16163,7 +16163,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>S27</t>
+          <t>S15</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -16518,17 +16518,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S180</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S146</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>S139717</t>
+          <t>S138724</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -16595,7 +16595,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>S36</t>
+          <t>S34</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -16883,7 +16883,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>S25</t>
+          <t>S8</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -16955,7 +16955,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>S76</t>
+          <t>S60</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -17027,7 +17027,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>S239</t>
+          <t>S162</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -17099,7 +17099,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -17238,17 +17238,17 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S180</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S118</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>S149210</t>
+          <t>S150270</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -17392,7 +17392,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>S184965</t>
+          <t>S187764</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -17459,7 +17459,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>S24</t>
+          <t>S22</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -17603,7 +17603,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>S10</t>
+          <t>S8</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -17819,7 +17819,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>S55</t>
+          <t>S36</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -18251,7 +18251,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S13</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -18688,7 +18688,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>S200005</t>
+          <t>S198650</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -18827,7 +18827,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>S31</t>
+          <t>S24</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">

</xml_diff>

<commit_message>
Updated requirements.txt and started implementing testing
</commit_message>
<xml_diff>
--- a/moduler/toolmonitor_data/results/RawDatabase.xlsx
+++ b/moduler/toolmonitor_data/results/RawDatabase.xlsx
@@ -1888,7 +1888,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>S20</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>S9</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>S6</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3112,7 +3112,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>S52</t>
+          <t>S39</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4932,7 +4932,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>S10000000</t>
+          <t>S00000000</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -4984,12 +4984,12 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>S0</t>
+          <t>S24</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>S203594</t>
+          <t>S197850</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -7432,7 +7432,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>S10</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -9755,7 +9755,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>S38</t>
+          <t>S33</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -9827,7 +9827,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>S129</t>
+          <t>S125</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -10115,7 +10115,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>S20</t>
+          <t>S17</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -14075,12 +14075,12 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S19</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>S217255</t>
+          <t>S217345</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -14435,7 +14435,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>S6</t>
+          <t>S5</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -14723,7 +14723,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>S85</t>
+          <t>S84</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -14867,7 +14867,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>S28</t>
+          <t>S27</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -14939,12 +14939,12 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>S34</t>
+          <t>S56</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>S180165</t>
+          <t>S152416</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -15371,7 +15371,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>S45</t>
+          <t>S44</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -18827,7 +18827,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>S24</t>
+          <t>S23</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">

</xml_diff>